<commit_message>
New Functionalities Added to generate MERGE and Insert macro
</commit_message>
<xml_diff>
--- a/mappings/D_OPCO_DDL_mapping.xlsx
+++ b/mappings/D_OPCO_DDL_mapping.xlsx
@@ -174,6 +174,11 @@
     <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <t>For incremental models, specify comma-separated column names to use as unique keys</t>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <t>Set to Y to exclude audit columns and unique key combination in the minus logic</t>
       </text>
     </comment>
   </commentList>
@@ -484,7 +489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,181 +560,186 @@
       </c>
       <c r="B7" t="n"/>
     </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>MINUS_LOGIC_REQUIRED</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>S.NO</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>TargetColumn</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Source Table</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>Logic/Mapping/Constant Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>OPCO_ID</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DATA_SRC</t>
+          <t>OPCO_ID</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CREATE_BY</t>
+          <t>DATA_SRC</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CREATE_PGM</t>
+          <t>CREATE_BY</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>UPDATE_BY</t>
+          <t>CREATE_PGM</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>UPDATE_PGM</t>
+          <t>UPDATE_BY</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OPCO_CD</t>
+          <t>UPDATE_PGM</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>OPCO_DSC</t>
+          <t>OPCO_CD</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RPT_OPCO_DSC</t>
+          <t>OPCO_DSC</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RPT_OPCO_ABBRV</t>
+          <t>RPT_OPCO_DSC</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>RPT_OPCO_ABBRV</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>11</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>TBA_ACTIVE_FLG</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>JOIN_TABLES</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>Join Type</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
         <is>
           <t>Table Type</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr">
+      <c r="C24" s="3" t="inlineStr">
         <is>
           <t>Source Name</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr">
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>Table Name</t>
         </is>
       </c>
-      <c r="E23" s="3" t="inlineStr">
+      <c r="E24" s="3" t="inlineStr">
         <is>
           <t>Alias</t>
         </is>
       </c>
-      <c r="F23" s="3" t="inlineStr">
+      <c r="F24" s="3" t="inlineStr">
         <is>
           <t>Join Condition</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>LEFT</t>
         </is>
       </c>
     </row>
@@ -761,15 +771,22 @@
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>LEFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>WHERE_CONDITIONS</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>GROUP BY</t>
         </is>
@@ -777,22 +794,19 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B30:F30"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B33:F33"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
     <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"incremental,truncate_load"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"LEFT,INNER"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B24" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"source,ref"</formula1>
+    <dataValidation sqref="B8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Y,N"</formula1>
     </dataValidation>
     <dataValidation sqref="A25" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
@@ -816,6 +830,12 @@
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
     <dataValidation sqref="B28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"source,ref"</formula1>
+    </dataValidation>
+    <dataValidation sqref="A29" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"LEFT,INNER"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B29" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
dag  genetor new functionaliy
</commit_message>
<xml_diff>
--- a/mappings/D_OPCO_DDL_mapping.xlsx
+++ b/mappings/D_OPCO_DDL_mapping.xlsx
@@ -179,6 +179,11 @@
     <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <t>Set to Y to exclude audit columns and unique key combination in the minus logic</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <t>Set to Y to set true tag for transient model property</t>
       </text>
     </comment>
   </commentList>
@@ -489,7 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,181 +577,186 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>TRANSIENT_TABLE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>S.NO</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>TargetColumn</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Source Table</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Logic/Mapping/Constant Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>OPCO_ID</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DATA_SRC</t>
+          <t>OPCO_ID</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CREATE_BY</t>
+          <t>DATA_SRC</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CREATE_PGM</t>
+          <t>CREATE_BY</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>UPDATE_BY</t>
+          <t>CREATE_PGM</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>UPDATE_PGM</t>
+          <t>UPDATE_BY</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>OPCO_CD</t>
+          <t>UPDATE_PGM</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>OPCO_DSC</t>
+          <t>OPCO_CD</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RPT_OPCO_DSC</t>
+          <t>OPCO_DSC</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RPT_OPCO_ABBRV</t>
+          <t>RPT_OPCO_DSC</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>RPT_OPCO_ABBRV</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>11</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>TBA_ACTIVE_FLG</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>JOIN_TABLES</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Join Type</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B25" s="3" t="inlineStr">
         <is>
           <t>Table Type</t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr">
+      <c r="C25" s="3" t="inlineStr">
         <is>
           <t>Source Name</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
+      <c r="D25" s="3" t="inlineStr">
         <is>
           <t>Table Name</t>
         </is>
       </c>
-      <c r="E24" s="3" t="inlineStr">
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t>Alias</t>
         </is>
       </c>
-      <c r="F24" s="3" t="inlineStr">
+      <c r="F25" s="3" t="inlineStr">
         <is>
           <t>Join Condition</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>LEFT</t>
         </is>
       </c>
     </row>
@@ -778,15 +788,22 @@
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>LEFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>WHERE_CONDITIONS</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>GROUP BY</t>
         </is>
@@ -794,25 +811,22 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B32:F32"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
     <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"incremental,truncate_load"</formula1>
+      <formula1>"incremental,truncate_load,lnd_load"</formula1>
     </dataValidation>
     <dataValidation sqref="B8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation sqref="A25" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"LEFT,INNER"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B25" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"source,ref"</formula1>
+    <dataValidation sqref="B9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Y,N"</formula1>
     </dataValidation>
     <dataValidation sqref="A26" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
@@ -836,6 +850,12 @@
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
     <dataValidation sqref="B29" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"source,ref"</formula1>
+    </dataValidation>
+    <dataValidation sqref="A30" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"LEFT,INNER"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B30" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1005,7 +1025,7 @@
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>CORE_DEV_MANAGER_ROLE</t>
+          <t>REV_GROWTH_MGMT_DEV_EDITOR_ROLE</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
@@ -1022,7 +1042,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>CORE_DEV_SELECT_WH</t>
+          <t>REV_GROWTH_MGMT_DEV_LOAD_WH</t>
         </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
@@ -1039,7 +1059,7 @@
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>CORE_DEV_DB</t>
+          <t>REV_GROWTH_MGMT_DEV_DB</t>
         </is>
       </c>
       <c r="C17" s="5" t="inlineStr">

</xml_diff>

<commit_message>
Cleaning Up the UI and optimisation in UI loop
</commit_message>
<xml_diff>
--- a/mappings/D_OPCO_DDL_mapping.xlsx
+++ b/mappings/D_OPCO_DDL_mapping.xlsx
@@ -811,56 +811,56 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="B32:F32"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="B34:F34"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
-    <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"incremental,truncate_load,lnd_load"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation sqref="A26" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A26" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
-    <dataValidation sqref="B26" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B26" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
-    <dataValidation sqref="A27" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A27" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
-    <dataValidation sqref="B27" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B27" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
-    <dataValidation sqref="A28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
-    <dataValidation sqref="B28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
-    <dataValidation sqref="A29" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A29" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
-    <dataValidation sqref="B29" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B29" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
-    <dataValidation sqref="A30" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A30" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"LEFT,INNER"</formula1>
     </dataValidation>
-    <dataValidation sqref="B30" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B30" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"source,ref"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1125,11 +1125,11 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"DATASET DEPENDENCY,CRON,SNS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>